<commit_message>
he vuelto a modificar algo
</commit_message>
<xml_diff>
--- a/Excel prueba.xlsx
+++ b/Excel prueba.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Curso Mañana\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>MESES</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Diferencia</t>
+  </si>
+  <si>
+    <t>GRÁFICO</t>
   </si>
 </sst>
 </file>
@@ -639,11 +642,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="230064816"/>
-        <c:axId val="230065208"/>
+        <c:axId val="193790832"/>
+        <c:axId val="194110800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="230064816"/>
+        <c:axId val="193790832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -685,7 +688,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="230065208"/>
+        <c:crossAx val="194110800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -693,7 +696,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="230065208"/>
+        <c:axId val="194110800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,7 +746,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="230064816"/>
+        <c:crossAx val="193790832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1028,11 +1031,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="306163736"/>
-        <c:axId val="306163344"/>
+        <c:axId val="194280624"/>
+        <c:axId val="194642880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="306163736"/>
+        <c:axId val="194280624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1075,7 +1078,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="306163344"/>
+        <c:crossAx val="194642880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1083,7 +1086,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="306163344"/>
+        <c:axId val="194642880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1134,7 +1137,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="306163736"/>
+        <c:crossAx val="194280624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1479,11 +1482,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="311402552"/>
-        <c:axId val="311402944"/>
+        <c:axId val="194607512"/>
+        <c:axId val="194626640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="311402552"/>
+        <c:axId val="194607512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1526,7 +1529,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="311402944"/>
+        <c:crossAx val="194626640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1534,7 +1537,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="311402944"/>
+        <c:axId val="194626640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1585,7 +1588,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="311402552"/>
+        <c:crossAx val="194607512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1842,8 +1845,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="311735176"/>
-        <c:axId val="311734784"/>
+        <c:axId val="194265888"/>
+        <c:axId val="193367776"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1934,7 +1937,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="311735176"/>
+        <c:axId val="194265888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1977,7 +1980,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="311734784"/>
+        <c:crossAx val="193367776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1985,7 +1988,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="311734784"/>
+        <c:axId val="193367776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2036,7 +2039,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="311735176"/>
+        <c:crossAx val="194265888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4918,11 +4921,11 @@
         <v>50</v>
       </c>
       <c r="O5" s="11">
-        <f t="shared" ref="O4:O12" si="0">SUM(C5:N5)</f>
+        <f t="shared" ref="O5:O12" si="0">SUM(C5:N5)</f>
         <v>600</v>
       </c>
       <c r="P5" s="12">
-        <f t="shared" ref="P4:P13" si="1">O5/$O$12</f>
+        <f t="shared" ref="P5:P13" si="1">O5/$O$12</f>
         <v>0.21849963583394028</v>
       </c>
     </row>
@@ -5575,10 +5578,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O4"/>
+  <dimension ref="B1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5701,6 +5704,11 @@
         <v>14454</v>
       </c>
     </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>